<commit_message>
weekly commit after report generation for the week
</commit_message>
<xml_diff>
--- a/3_output/y2025_w32_weekly_report_output.xlsx
+++ b/3_output/y2025_w32_weekly_report_output.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="315">
   <si>
     <t xml:space="preserve">Year</t>
   </si>
@@ -785,159 +785,147 @@
     <t xml:space="preserve">abund_Tarsalis</t>
   </si>
   <si>
+    <t xml:space="preserve">pir_Pipiens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pir_Tarsalis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vi_Pipiens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vi_Tarsalis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vi_All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">week</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vi_NW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vi_hx_NW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vi_NE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vi_hx_NE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vi_SE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vi_hx_SE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vi_SW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vi_hx_SW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vi_FC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vi_hx_FC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vi_LV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vi_BE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vi_BC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">collected_Pipiens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">collected_Tarsalis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">collected_All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trap_L</t>
+  </si>
+  <si>
     <t xml:space="preserve">abund_All</t>
   </si>
   <si>
-    <t xml:space="preserve">pir_Pipiens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pir_Tarsalis</t>
+    <t xml:space="preserve">abund_NW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abund_hx_NW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abund_NE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abund_hx_NE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abund_SE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abund_hx_SE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abund_SW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abund_hx_SW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abund_FC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abund_hx_FC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abund_LV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abund_BE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">abund_BC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">examined_Pipiens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">examined_Tarsalis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">examined_All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pool_Pipiens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pool_Tarsalis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pool_all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pos_pool_Pipiens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pos_pool_Tarsalis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pos_pool_all</t>
   </si>
   <si>
     <t xml:space="preserve">pir_All</t>
   </si>
   <si>
-    <t xml:space="preserve">vi_Pipiens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vi_Tarsalis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vi_All</t>
-  </si>
-  <si>
-    <t xml:space="preserve">week</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vi_NW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vi_hx_NW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vi_NE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vi_hx_NE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vi_SE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vi_hx_SE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vi_SW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vi_hx_SW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vi_FC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vi_hx_FC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vi_LV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vi_hx_LV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vi_BE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vi_hx_BE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vi_BC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vi_hx_BC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">collected_Pipiens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">collected_Tarsalis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">collected_All</t>
-  </si>
-  <si>
-    <t xml:space="preserve">trap_L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abund_NW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abund_hx_NW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abund_NE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abund_hx_NE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abund_SE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abund_hx_SE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abund_SW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abund_hx_SW</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abund_FC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abund_hx_FC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abund_LV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abund_hx_LV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abund_BE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abund_hx_BE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abund_BC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abund_hx_BC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">examined_Pipiens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">examined_Tarsalis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">examined_All</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pool_Pipiens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pool_Tarsalis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pos_pool_Pipiens</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pos_pool_Tarsalis</t>
-  </si>
-  <si>
     <t xml:space="preserve">pir_NW</t>
   </si>
   <si>
@@ -971,19 +959,10 @@
     <t xml:space="preserve">pir_LV</t>
   </si>
   <si>
-    <t xml:space="preserve">pir_hx_LV</t>
-  </si>
-  <si>
     <t xml:space="preserve">pir_BE</t>
   </si>
   <si>
-    <t xml:space="preserve">pir_hx_BE</t>
-  </si>
-  <si>
     <t xml:space="preserve">pir_BC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pir_hx_BC</t>
   </si>
 </sst>
 </file>
@@ -9074,12 +9053,6 @@
       <c r="H1" t="s">
         <v>259</v>
       </c>
-      <c r="I1" t="s">
-        <v>260</v>
-      </c>
-      <c r="J1" t="s">
-        <v>261</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
@@ -9092,24 +9065,18 @@
         <v>32.6667</v>
       </c>
       <c r="D2" t="n">
-        <v>41.4444</v>
+        <v>0.0119</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0119</v>
+        <v>0.0073</v>
       </c>
       <c r="F2" t="n">
-        <v>0.0073</v>
+        <v>0.1</v>
       </c>
       <c r="G2" t="n">
-        <v>0.0094</v>
+        <v>0.24</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="I2" t="n">
-        <v>0.24</v>
-      </c>
-      <c r="J2" t="n">
         <v>0.39</v>
       </c>
     </row>
@@ -9124,24 +9091,18 @@
         <v>22.8</v>
       </c>
       <c r="D3" t="n">
-        <v>39.3</v>
+        <v>0.0122</v>
       </c>
       <c r="E3" t="n">
-        <v>0.0122</v>
+        <v>0.0046</v>
       </c>
       <c r="F3" t="n">
-        <v>0.0046</v>
+        <v>0.2</v>
       </c>
       <c r="G3" t="n">
-        <v>0.0089</v>
+        <v>0.1</v>
       </c>
       <c r="H3" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="I3" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="J3" t="n">
         <v>0.35</v>
       </c>
     </row>
@@ -9156,24 +9117,18 @@
         <v>25.5</v>
       </c>
       <c r="D4" t="n">
-        <v>31.0714</v>
+        <v>0.0163</v>
       </c>
       <c r="E4" t="n">
-        <v>0.0163</v>
+        <v>0.0098</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0098</v>
+        <v>0.09</v>
       </c>
       <c r="G4" t="n">
-        <v>0.0134</v>
+        <v>0.25</v>
       </c>
       <c r="H4" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="I4" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="J4" t="n">
         <v>0.42</v>
       </c>
     </row>
@@ -9188,24 +9143,18 @@
         <v>24.5556</v>
       </c>
       <c r="D5" t="n">
-        <v>34.3333</v>
+        <v>0.0179</v>
       </c>
       <c r="E5" t="n">
-        <v>0.0179</v>
+        <v>0.0044</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0044</v>
+        <v>0.18</v>
       </c>
       <c r="G5" t="n">
-        <v>0.0106</v>
+        <v>0.11</v>
       </c>
       <c r="H5" t="n">
-        <v>0.18</v>
-      </c>
-      <c r="I5" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="J5" t="n">
         <v>0.36</v>
       </c>
     </row>
@@ -9220,120 +9169,106 @@
         <v>26.1905</v>
       </c>
       <c r="D6" t="n">
-        <v>35.9524</v>
+        <v>0.0155</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0155</v>
+        <v>0.0072</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0072</v>
+        <v>0.15</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0111</v>
+        <v>0.19</v>
       </c>
       <c r="H6" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="I6" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="J6" t="n">
         <v>0.4</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" t="n">
-        <v>7</v>
-      </c>
-      <c r="C7" t="n">
-        <v>56.6667</v>
-      </c>
-      <c r="D7" t="n">
-        <v>63.6667</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>0.0063</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0.0056</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0.36</v>
-      </c>
-      <c r="J7" t="n">
-        <v>0.36</v>
-      </c>
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>148</v>
+        <v>39</v>
       </c>
       <c r="B8" t="n">
-        <v>3.3</v>
+        <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>74.7</v>
+        <v>56.6667</v>
       </c>
       <c r="D8" t="n">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>0</v>
+        <v>0.0063</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0077</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0074</v>
+        <v>0.36</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" t="n">
-        <v>0.58</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.58</v>
+        <v>0.36</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B9" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="C9" t="n">
+        <v>74.7</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.0077</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.58</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B10" t="n">
         <v>1.8</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C10" t="n">
         <v>32.4</v>
       </c>
-      <c r="D9" t="n">
-        <v>34.2</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="n">
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
         <v>0.0194</v>
       </c>
-      <c r="G9" t="n">
-        <v>0.0194</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" t="n">
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
         <v>0.63</v>
       </c>
-      <c r="J9" t="n">
+      <c r="H10" t="n">
         <v>0.66</v>
       </c>
     </row>
@@ -9353,55 +9288,46 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
+        <v>260</v>
+      </c>
+      <c r="B1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C1" t="s">
         <v>262</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>263</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>264</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>265</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>266</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>267</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>268</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>269</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>270</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>271</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>272</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>273</v>
-      </c>
-      <c r="M1" t="s">
-        <v>274</v>
-      </c>
-      <c r="N1" t="s">
-        <v>275</v>
-      </c>
-      <c r="O1" t="s">
-        <v>276</v>
-      </c>
-      <c r="P1" t="s">
-        <v>277</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="2">
@@ -9444,14 +9370,7 @@
       <c r="M2" t="n">
         <v>0</v>
       </c>
-      <c r="N2" t="n">
-        <v>0</v>
-      </c>
-      <c r="O2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2"/>
-      <c r="Q2"/>
+      <c r="N2"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -9493,16 +9412,7 @@
       <c r="M3" t="n">
         <v>0</v>
       </c>
-      <c r="N3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3"/>
-      <c r="Q3" t="n">
-        <v>0</v>
-      </c>
+      <c r="N3"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -9547,15 +9457,6 @@
       <c r="N4" t="n">
         <v>0</v>
       </c>
-      <c r="O4" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -9598,16 +9499,7 @@
         <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" t="n">
         <v>0.2</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -9648,19 +9540,10 @@
         <v>0.16</v>
       </c>
       <c r="M6" t="n">
-        <v>0.15</v>
+        <v>0.22</v>
       </c>
       <c r="N6" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="O6" t="n">
         <v>0.3</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -9701,19 +9584,10 @@
         <v>0.55</v>
       </c>
       <c r="M7" t="n">
-        <v>0.08</v>
+        <v>0.44</v>
       </c>
       <c r="N7" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0.56</v>
-      </c>
-      <c r="P7" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -9754,19 +9628,10 @@
         <v>1.03</v>
       </c>
       <c r="M8" t="n">
-        <v>0.36</v>
+        <v>1.01</v>
       </c>
       <c r="N8" t="n">
-        <v>1.01</v>
-      </c>
-      <c r="O8" t="n">
-        <v>0.46</v>
-      </c>
-      <c r="P8" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>0.18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -9807,19 +9672,10 @@
         <v>0.76</v>
       </c>
       <c r="M9" t="n">
-        <v>1.44</v>
+        <v>0.56</v>
       </c>
       <c r="N9" t="n">
-        <v>0.56</v>
-      </c>
-      <c r="O9" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="P9" t="n">
         <v>0.9</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>0.09</v>
       </c>
     </row>
     <row r="10">
@@ -9863,16 +9719,7 @@
         <v>0.45</v>
       </c>
       <c r="N10" t="n">
-        <v>0.45</v>
-      </c>
-      <c r="O10" t="n">
-        <v>0.24</v>
-      </c>
-      <c r="P10" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -9913,19 +9760,10 @@
         <v>0.36</v>
       </c>
       <c r="M11" t="n">
-        <v>0.55</v>
+        <v>0.58</v>
       </c>
       <c r="N11" t="n">
-        <v>0.58</v>
-      </c>
-      <c r="O11" t="n">
-        <v>0.73</v>
-      </c>
-      <c r="P11" t="n">
         <v>0.66</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>0.16</v>
       </c>
     </row>
     <row r="12">
@@ -9953,17 +9791,8 @@
         <v>0.35</v>
       </c>
       <c r="L12"/>
-      <c r="M12" t="n">
-        <v>0.51</v>
-      </c>
+      <c r="M12"/>
       <c r="N12"/>
-      <c r="O12" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="P12"/>
-      <c r="Q12" t="n">
-        <v>0.1</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -9990,17 +9819,8 @@
         <v>0.36</v>
       </c>
       <c r="L13"/>
-      <c r="M13" t="n">
-        <v>0.3</v>
-      </c>
+      <c r="M13"/>
       <c r="N13"/>
-      <c r="O13" t="n">
-        <v>0.48</v>
-      </c>
-      <c r="P13"/>
-      <c r="Q13" t="n">
-        <v>0.1</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -10027,17 +9847,8 @@
         <v>0.27</v>
       </c>
       <c r="L14"/>
-      <c r="M14" t="n">
-        <v>0.28</v>
-      </c>
+      <c r="M14"/>
       <c r="N14"/>
-      <c r="O14" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="P14"/>
-      <c r="Q14" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -10064,15 +9875,8 @@
         <v>0.08</v>
       </c>
       <c r="L15"/>
-      <c r="M15" t="n">
-        <v>0.15</v>
-      </c>
+      <c r="M15"/>
       <c r="N15"/>
-      <c r="O15"/>
-      <c r="P15"/>
-      <c r="Q15" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -10101,11 +9905,6 @@
       <c r="L16"/>
       <c r="M16"/>
       <c r="N16"/>
-      <c r="O16"/>
-      <c r="P16"/>
-      <c r="Q16" t="n">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -10126,16 +9925,16 @@
         <v>252</v>
       </c>
       <c r="B1" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="C1" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D1" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="E1" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="F1" t="s">
         <v>253</v>
@@ -10144,7 +9943,7 @@
         <v>254</v>
       </c>
       <c r="H1" t="s">
-        <v>255</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2">
@@ -10164,13 +9963,13 @@
         <v>9</v>
       </c>
       <c r="F2" t="n">
-        <v>8.7778</v>
+        <v>8.78</v>
       </c>
       <c r="G2" t="n">
-        <v>32.6667</v>
+        <v>32.67</v>
       </c>
       <c r="H2" t="n">
-        <v>41.4444</v>
+        <v>41.44</v>
       </c>
     </row>
     <row r="3">
@@ -10216,13 +10015,13 @@
         <v>14</v>
       </c>
       <c r="F4" t="n">
-        <v>5.5714</v>
+        <v>5.57</v>
       </c>
       <c r="G4" t="n">
         <v>25.5</v>
       </c>
       <c r="H4" t="n">
-        <v>31.0714</v>
+        <v>31.07</v>
       </c>
     </row>
     <row r="5">
@@ -10242,13 +10041,13 @@
         <v>9</v>
       </c>
       <c r="F5" t="n">
-        <v>9.7778</v>
+        <v>9.78</v>
       </c>
       <c r="G5" t="n">
-        <v>24.5556</v>
+        <v>24.56</v>
       </c>
       <c r="H5" t="n">
-        <v>34.3333</v>
+        <v>34.33</v>
       </c>
     </row>
     <row r="6">
@@ -10268,90 +10067,100 @@
         <v>42</v>
       </c>
       <c r="F6" t="n">
-        <v>9.7619</v>
+        <v>9.76</v>
       </c>
       <c r="G6" t="n">
-        <v>26.1905</v>
+        <v>26.19</v>
       </c>
       <c r="H6" t="n">
-        <v>35.9524</v>
+        <v>35.95</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" t="n">
-        <v>42</v>
-      </c>
-      <c r="C7" t="n">
-        <v>340</v>
-      </c>
-      <c r="D7" t="n">
-        <v>382</v>
-      </c>
-      <c r="E7" t="n">
-        <v>6</v>
-      </c>
-      <c r="F7" t="n">
-        <v>7</v>
-      </c>
-      <c r="G7" t="n">
-        <v>56.6667</v>
-      </c>
-      <c r="H7" t="n">
-        <v>63.6667</v>
-      </c>
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>148</v>
+        <v>39</v>
       </c>
       <c r="B8" t="n">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C8" t="n">
-        <v>747</v>
+        <v>340</v>
       </c>
       <c r="D8" t="n">
-        <v>780</v>
+        <v>382</v>
       </c>
       <c r="E8" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="F8" t="n">
-        <v>3.3</v>
+        <v>7</v>
       </c>
       <c r="G8" t="n">
-        <v>74.7</v>
+        <v>56.67</v>
       </c>
       <c r="H8" t="n">
-        <v>78</v>
+        <v>63.67</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B9" t="n">
+        <v>33</v>
+      </c>
+      <c r="C9" t="n">
+        <v>747</v>
+      </c>
+      <c r="D9" t="n">
+        <v>780</v>
+      </c>
+      <c r="E9" t="n">
+        <v>10</v>
+      </c>
+      <c r="F9" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="G9" t="n">
+        <v>74.7</v>
+      </c>
+      <c r="H9" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B10" t="n">
         <v>9</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C10" t="n">
         <v>162</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D10" t="n">
         <v>171</v>
       </c>
-      <c r="E9" t="n">
+      <c r="E10" t="n">
         <v>5</v>
       </c>
-      <c r="F9" t="n">
+      <c r="F10" t="n">
         <v>1.8</v>
       </c>
-      <c r="G9" t="n">
+      <c r="G10" t="n">
         <v>32.4</v>
       </c>
-      <c r="H9" t="n">
+      <c r="H10" t="n">
         <v>34.2</v>
       </c>
     </row>
@@ -10371,55 +10180,46 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B1" t="s">
+        <v>279</v>
+      </c>
+      <c r="C1" t="s">
+        <v>280</v>
+      </c>
+      <c r="D1" t="s">
+        <v>281</v>
+      </c>
+      <c r="E1" t="s">
+        <v>282</v>
+      </c>
+      <c r="F1" t="s">
         <v>283</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>284</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>285</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>286</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>287</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>288</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>289</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>290</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>291</v>
-      </c>
-      <c r="K1" t="s">
-        <v>292</v>
-      </c>
-      <c r="L1" t="s">
-        <v>293</v>
-      </c>
-      <c r="M1" t="s">
-        <v>294</v>
-      </c>
-      <c r="N1" t="s">
-        <v>295</v>
-      </c>
-      <c r="O1" t="s">
-        <v>296</v>
-      </c>
-      <c r="P1" t="s">
-        <v>297</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="2">
@@ -10460,16 +10260,9 @@
         <v>2.33</v>
       </c>
       <c r="M2" t="n">
-        <v>18.58</v>
-      </c>
-      <c r="N2" t="n">
         <v>3.1</v>
       </c>
-      <c r="O2" t="n">
-        <v>12</v>
-      </c>
-      <c r="P2"/>
-      <c r="Q2"/>
+      <c r="N2"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -10509,18 +10302,9 @@
         <v>21.6</v>
       </c>
       <c r="M3" t="n">
-        <v>24.37</v>
-      </c>
-      <c r="N3" t="n">
         <v>17.4</v>
       </c>
-      <c r="O3" t="n">
-        <v>16.87</v>
-      </c>
-      <c r="P3"/>
-      <c r="Q3" t="n">
-        <v>17.42</v>
-      </c>
+      <c r="N3"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -10560,19 +10344,10 @@
         <v>99.67</v>
       </c>
       <c r="M4" t="n">
-        <v>49.65</v>
+        <v>7</v>
       </c>
       <c r="N4" t="n">
-        <v>7</v>
-      </c>
-      <c r="O4" t="n">
-        <v>44.32</v>
-      </c>
-      <c r="P4" t="n">
         <v>42.4</v>
-      </c>
-      <c r="Q4" t="n">
-        <v>17.7</v>
       </c>
     </row>
     <row r="5">
@@ -10613,19 +10388,10 @@
         <v>87.17</v>
       </c>
       <c r="M5" t="n">
-        <v>131.98</v>
+        <v>22.7</v>
       </c>
       <c r="N5" t="n">
-        <v>22.7</v>
-      </c>
-      <c r="O5" t="n">
-        <v>157.1</v>
-      </c>
-      <c r="P5" t="n">
         <v>25.5</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>21.65</v>
       </c>
     </row>
     <row r="6">
@@ -10666,19 +10432,10 @@
         <v>183</v>
       </c>
       <c r="M6" t="n">
-        <v>364.08</v>
+        <v>59.11</v>
       </c>
       <c r="N6" t="n">
-        <v>59.11</v>
-      </c>
-      <c r="O6" t="n">
-        <v>165.36</v>
-      </c>
-      <c r="P6" t="n">
         <v>58</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>40.5</v>
       </c>
     </row>
     <row r="7">
@@ -10719,19 +10476,10 @@
         <v>97.5</v>
       </c>
       <c r="M7" t="n">
-        <v>216.67</v>
+        <v>84.6</v>
       </c>
       <c r="N7" t="n">
-        <v>84.6</v>
-      </c>
-      <c r="O7" t="n">
-        <v>240.25</v>
-      </c>
-      <c r="P7" t="n">
         <v>126.8</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>38.6</v>
       </c>
     </row>
     <row r="8">
@@ -10772,19 +10520,10 @@
         <v>79.33</v>
       </c>
       <c r="M8" t="n">
-        <v>250.81</v>
+        <v>74</v>
       </c>
       <c r="N8" t="n">
-        <v>74</v>
-      </c>
-      <c r="O8" t="n">
-        <v>197.8</v>
-      </c>
-      <c r="P8" t="n">
         <v>145.6</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>44.2</v>
       </c>
     </row>
     <row r="9">
@@ -10825,19 +10564,10 @@
         <v>97</v>
       </c>
       <c r="M9" t="n">
-        <v>206.52</v>
+        <v>55.8</v>
       </c>
       <c r="N9" t="n">
-        <v>55.8</v>
-      </c>
-      <c r="O9" t="n">
-        <v>96.57</v>
-      </c>
-      <c r="P9" t="n">
         <v>53.2</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>44.45</v>
       </c>
     </row>
     <row r="10">
@@ -10878,19 +10608,10 @@
         <v>40.83</v>
       </c>
       <c r="M10" t="n">
-        <v>169.06</v>
+        <v>43.3</v>
       </c>
       <c r="N10" t="n">
-        <v>43.3</v>
-      </c>
-      <c r="O10" t="n">
-        <v>78.33</v>
-      </c>
-      <c r="P10" t="n">
         <v>10.6</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>42.65</v>
       </c>
     </row>
     <row r="11">
@@ -10931,19 +10652,10 @@
         <v>63.67</v>
       </c>
       <c r="M11" t="n">
-        <v>97.8</v>
+        <v>78</v>
       </c>
       <c r="N11" t="n">
-        <v>78</v>
-      </c>
-      <c r="O11" t="n">
-        <v>93.02</v>
-      </c>
-      <c r="P11" t="n">
         <v>34.2</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>31.6</v>
       </c>
     </row>
     <row r="12">
@@ -10971,17 +10683,8 @@
         <v>64.41</v>
       </c>
       <c r="L12"/>
-      <c r="M12" t="n">
-        <v>82.97</v>
-      </c>
+      <c r="M12"/>
       <c r="N12"/>
-      <c r="O12" t="n">
-        <v>51.01</v>
-      </c>
-      <c r="P12"/>
-      <c r="Q12" t="n">
-        <v>22.9</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -11008,17 +10711,8 @@
         <v>56.95</v>
       </c>
       <c r="L13"/>
-      <c r="M13" t="n">
-        <v>80.5</v>
-      </c>
+      <c r="M13"/>
       <c r="N13"/>
-      <c r="O13" t="n">
-        <v>42.56</v>
-      </c>
-      <c r="P13"/>
-      <c r="Q13" t="n">
-        <v>18.65</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -11045,17 +10739,8 @@
         <v>30.16</v>
       </c>
       <c r="L14"/>
-      <c r="M14" t="n">
-        <v>39.9</v>
-      </c>
+      <c r="M14"/>
       <c r="N14"/>
-      <c r="O14" t="n">
-        <v>22.41</v>
-      </c>
-      <c r="P14"/>
-      <c r="Q14" t="n">
-        <v>9.13</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -11082,15 +10767,8 @@
         <v>20.13</v>
       </c>
       <c r="L15"/>
-      <c r="M15" t="n">
-        <v>21.97</v>
-      </c>
+      <c r="M15"/>
       <c r="N15"/>
-      <c r="O15"/>
-      <c r="P15"/>
-      <c r="Q15" t="n">
-        <v>5.45</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -11119,11 +10797,6 @@
       <c r="L16"/>
       <c r="M16"/>
       <c r="N16"/>
-      <c r="O16"/>
-      <c r="P16"/>
-      <c r="Q16" t="n">
-        <v>7</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11144,34 +10817,40 @@
         <v>252</v>
       </c>
       <c r="B1" t="s">
+        <v>292</v>
+      </c>
+      <c r="C1" t="s">
+        <v>293</v>
+      </c>
+      <c r="D1" t="s">
+        <v>294</v>
+      </c>
+      <c r="E1" t="s">
+        <v>295</v>
+      </c>
+      <c r="F1" t="s">
+        <v>296</v>
+      </c>
+      <c r="G1" t="s">
+        <v>297</v>
+      </c>
+      <c r="H1" t="s">
+        <v>298</v>
+      </c>
+      <c r="I1" t="s">
         <v>299</v>
       </c>
-      <c r="C1" t="s">
+      <c r="J1" t="s">
         <v>300</v>
       </c>
-      <c r="D1" t="s">
+      <c r="K1" t="s">
+        <v>255</v>
+      </c>
+      <c r="L1" t="s">
+        <v>256</v>
+      </c>
+      <c r="M1" t="s">
         <v>301</v>
-      </c>
-      <c r="E1" t="s">
-        <v>302</v>
-      </c>
-      <c r="F1" t="s">
-        <v>303</v>
-      </c>
-      <c r="G1" t="s">
-        <v>304</v>
-      </c>
-      <c r="H1" t="s">
-        <v>305</v>
-      </c>
-      <c r="I1" t="s">
-        <v>256</v>
-      </c>
-      <c r="J1" t="s">
-        <v>257</v>
-      </c>
-      <c r="K1" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="2">
@@ -11194,18 +10873,24 @@
         <v>11</v>
       </c>
       <c r="G2" t="n">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="H2" t="n">
         <v>2</v>
       </c>
       <c r="I2" t="n">
+        <v>2</v>
+      </c>
+      <c r="J2" t="n">
+        <v>4</v>
+      </c>
+      <c r="K2" t="n">
         <v>11.9</v>
       </c>
-      <c r="J2" t="n">
+      <c r="L2" t="n">
         <v>7.3</v>
       </c>
-      <c r="K2" t="n">
+      <c r="M2" t="n">
         <v>9.4</v>
       </c>
     </row>
@@ -11229,18 +10914,24 @@
         <v>10</v>
       </c>
       <c r="G3" t="n">
+        <v>24</v>
+      </c>
+      <c r="H3" t="n">
         <v>3</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>1</v>
       </c>
-      <c r="I3" t="n">
+      <c r="J3" t="n">
+        <v>4</v>
+      </c>
+      <c r="K3" t="n">
         <v>12.2</v>
       </c>
-      <c r="J3" t="n">
+      <c r="L3" t="n">
         <v>4.6</v>
       </c>
-      <c r="K3" t="n">
+      <c r="M3" t="n">
         <v>8.9</v>
       </c>
     </row>
@@ -11264,18 +10955,24 @@
         <v>15</v>
       </c>
       <c r="G4" t="n">
+        <v>35</v>
+      </c>
+      <c r="H4" t="n">
         <v>5</v>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>3</v>
       </c>
-      <c r="I4" t="n">
+      <c r="J4" t="n">
+        <v>8</v>
+      </c>
+      <c r="K4" t="n">
         <v>16.3</v>
       </c>
-      <c r="J4" t="n">
+      <c r="L4" t="n">
         <v>9.8</v>
       </c>
-      <c r="K4" t="n">
+      <c r="M4" t="n">
         <v>13.4</v>
       </c>
     </row>
@@ -11299,18 +10996,24 @@
         <v>9</v>
       </c>
       <c r="G5" t="n">
+        <v>18</v>
+      </c>
+      <c r="H5" t="n">
         <v>3</v>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>1</v>
       </c>
-      <c r="I5" t="n">
+      <c r="J5" t="n">
+        <v>4</v>
+      </c>
+      <c r="K5" t="n">
         <v>17.9</v>
       </c>
-      <c r="J5" t="n">
+      <c r="L5" t="n">
         <v>4.4</v>
       </c>
-      <c r="K5" t="n">
+      <c r="M5" t="n">
         <v>10.6</v>
       </c>
     </row>
@@ -11334,123 +11037,162 @@
         <v>45</v>
       </c>
       <c r="G6" t="n">
+        <v>98</v>
+      </c>
+      <c r="H6" t="n">
         <v>13</v>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>7</v>
       </c>
-      <c r="I6" t="n">
+      <c r="J6" t="n">
+        <v>20</v>
+      </c>
+      <c r="K6" t="n">
         <v>15.5</v>
       </c>
-      <c r="J6" t="n">
+      <c r="L6" t="n">
         <v>7.2</v>
       </c>
-      <c r="K6" t="n">
+      <c r="M6" t="n">
         <v>11.1</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" t="n">
-        <v>42</v>
-      </c>
-      <c r="C7" t="n">
-        <v>340</v>
-      </c>
-      <c r="D7" t="n">
-        <v>382</v>
-      </c>
-      <c r="E7" t="n">
-        <v>5</v>
-      </c>
-      <c r="F7" t="n">
-        <v>10</v>
-      </c>
-      <c r="G7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" t="n">
-        <v>2</v>
-      </c>
-      <c r="I7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" t="n">
-        <v>6.3</v>
-      </c>
-      <c r="K7" t="n">
-        <v>5.6</v>
-      </c>
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>148</v>
+        <v>39</v>
       </c>
       <c r="B8" t="n">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C8" t="n">
-        <v>747</v>
+        <v>340</v>
       </c>
       <c r="D8" t="n">
-        <v>780</v>
+        <v>382</v>
       </c>
       <c r="E8" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F8" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G8" t="n">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H8" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I8" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J8" t="n">
-        <v>7.7</v>
+        <v>2</v>
       </c>
       <c r="K8" t="n">
-        <v>7.4</v>
+        <v>0</v>
+      </c>
+      <c r="L8" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="M8" t="n">
+        <v>5.6</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B9" t="n">
+        <v>33</v>
+      </c>
+      <c r="C9" t="n">
+        <v>747</v>
+      </c>
+      <c r="D9" t="n">
+        <v>780</v>
+      </c>
+      <c r="E9" t="n">
+        <v>8</v>
+      </c>
+      <c r="F9" t="n">
         <v>19</v>
       </c>
-      <c r="B9" t="n">
+      <c r="G9" t="n">
+        <v>27</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
+        <v>5</v>
+      </c>
+      <c r="J9" t="n">
+        <v>5</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>7.7</v>
+      </c>
+      <c r="M9" t="n">
+        <v>7.4</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="n">
         <v>9</v>
       </c>
-      <c r="C9" t="n">
+      <c r="C10" t="n">
         <v>162</v>
       </c>
-      <c r="D9" t="n">
+      <c r="D10" t="n">
         <v>171</v>
       </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="n">
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
         <v>7</v>
       </c>
-      <c r="G9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" t="n">
+      <c r="G10" t="n">
+        <v>7</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" t="n">
         <v>3</v>
       </c>
-      <c r="I9" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" t="n">
+      <c r="J10" t="n">
+        <v>3</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
         <v>19.4</v>
       </c>
-      <c r="K9" t="n">
+      <c r="M10" t="n">
         <v>19.4</v>
       </c>
     </row>
@@ -11470,55 +11212,46 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B1" t="s">
+        <v>302</v>
+      </c>
+      <c r="C1" t="s">
+        <v>303</v>
+      </c>
+      <c r="D1" t="s">
+        <v>304</v>
+      </c>
+      <c r="E1" t="s">
+        <v>305</v>
+      </c>
+      <c r="F1" t="s">
         <v>306</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G1" t="s">
         <v>307</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>308</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>309</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>310</v>
       </c>
-      <c r="G1" t="s">
+      <c r="K1" t="s">
         <v>311</v>
       </c>
-      <c r="H1" t="s">
+      <c r="L1" t="s">
         <v>312</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" t="s">
         <v>313</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>314</v>
-      </c>
-      <c r="K1" t="s">
-        <v>315</v>
-      </c>
-      <c r="L1" t="s">
-        <v>316</v>
-      </c>
-      <c r="M1" t="s">
-        <v>317</v>
-      </c>
-      <c r="N1" t="s">
-        <v>318</v>
-      </c>
-      <c r="O1" t="s">
-        <v>319</v>
-      </c>
-      <c r="P1" t="s">
-        <v>320</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="2">
@@ -11564,15 +11297,6 @@
       <c r="N2" t="n">
         <v>0</v>
       </c>
-      <c r="O2" t="n">
-        <v>0</v>
-      </c>
-      <c r="P2" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -11615,15 +11339,6 @@
         <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>0</v>
-      </c>
-      <c r="O3" t="n">
-        <v>0</v>
-      </c>
-      <c r="P3" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11644,7 +11359,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0039</v>
+        <v>3.9</v>
       </c>
       <c r="G4" t="n">
         <v>0</v>
@@ -11656,7 +11371,7 @@
         <v>0</v>
       </c>
       <c r="J4" t="n">
-        <v>0.0024</v>
+        <v>2.4</v>
       </c>
       <c r="K4" t="n">
         <v>0</v>
@@ -11668,15 +11383,6 @@
         <v>0</v>
       </c>
       <c r="N4" t="n">
-        <v>0</v>
-      </c>
-      <c r="O4" t="n">
-        <v>0.0004</v>
-      </c>
-      <c r="P4" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -11685,7 +11391,7 @@
         <v>26</v>
       </c>
       <c r="B5" t="n">
-        <v>0.0165</v>
+        <v>16.5</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -11697,10 +11403,10 @@
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0029</v>
+        <v>2.9</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="H5" t="n">
         <v>0</v>
@@ -11709,28 +11415,19 @@
         <v>0</v>
       </c>
       <c r="J5" t="n">
-        <v>0.0024</v>
+        <v>2.4</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="L5" t="n">
-        <v>0.0019</v>
+        <v>1.9</v>
       </c>
       <c r="M5" t="n">
         <v>0</v>
       </c>
       <c r="N5" t="n">
-        <v>0</v>
-      </c>
-      <c r="O5" t="n">
-        <v>0</v>
-      </c>
-      <c r="P5" t="n">
-        <v>0.0079</v>
-      </c>
-      <c r="Q5" t="n">
-        <v>0</v>
+        <v>7.9</v>
       </c>
     </row>
     <row r="6">
@@ -11744,46 +11441,37 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0017</v>
+        <v>1.7</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0025</v>
+        <v>2.5</v>
       </c>
       <c r="G6" t="n">
-        <v>0.0001</v>
+        <v>0.09</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0018</v>
+        <v>1.8</v>
       </c>
       <c r="I6" t="n">
         <v>0</v>
       </c>
       <c r="J6" t="n">
-        <v>0.002</v>
+        <v>2</v>
       </c>
       <c r="K6" t="n">
-        <v>0.0001</v>
+        <v>0.06</v>
       </c>
       <c r="L6" t="n">
-        <v>0.0009</v>
+        <v>0.9</v>
       </c>
       <c r="M6" t="n">
-        <v>0.0001</v>
+        <v>3.7</v>
       </c>
       <c r="N6" t="n">
-        <v>0.0037</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0.0003</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0.0051</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>0</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="7">
@@ -11791,52 +11479,43 @@
         <v>28</v>
       </c>
       <c r="B7" t="n">
-        <v>0.0035</v>
+        <v>3.5</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0001</v>
+        <v>0.08</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0051</v>
+        <v>5.1</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0003</v>
+        <v>0.29</v>
       </c>
       <c r="F7" t="n">
-        <v>0.0058</v>
+        <v>5.8</v>
       </c>
       <c r="G7" t="n">
-        <v>0.0006</v>
+        <v>0.64</v>
       </c>
       <c r="H7" t="n">
-        <v>0.0032</v>
+        <v>3.2</v>
       </c>
       <c r="I7" t="n">
-        <v>0.0006</v>
+        <v>0.6</v>
       </c>
       <c r="J7" t="n">
-        <v>0.0051</v>
+        <v>5.1</v>
       </c>
       <c r="K7" t="n">
-        <v>0.0005</v>
+        <v>0.46</v>
       </c>
       <c r="L7" t="n">
-        <v>0.0056</v>
+        <v>5.6</v>
       </c>
       <c r="M7" t="n">
-        <v>0.0002</v>
+        <v>5.2</v>
       </c>
       <c r="N7" t="n">
-        <v>0.0052</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0.0016</v>
-      </c>
-      <c r="P7" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>0.0017</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -11844,52 +11523,43 @@
         <v>29</v>
       </c>
       <c r="B8" t="n">
-        <v>0.0078</v>
+        <v>7.8</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0009</v>
+        <v>0.89</v>
       </c>
       <c r="D8" t="n">
-        <v>0.0092</v>
+        <v>9.2</v>
       </c>
       <c r="E8" t="n">
-        <v>0.0009</v>
+        <v>0.91</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0146</v>
+        <v>14.6</v>
       </c>
       <c r="G8" t="n">
-        <v>0.0011</v>
+        <v>1.11</v>
       </c>
       <c r="H8" t="n">
-        <v>0.0102</v>
+        <v>10.2</v>
       </c>
       <c r="I8" t="n">
-        <v>0.001</v>
+        <v>0.95</v>
       </c>
       <c r="J8" t="n">
-        <v>0.0111</v>
+        <v>11.1</v>
       </c>
       <c r="K8" t="n">
-        <v>0.001</v>
+        <v>1</v>
       </c>
       <c r="L8" t="n">
-        <v>0.013</v>
+        <v>13</v>
       </c>
       <c r="M8" t="n">
-        <v>0.0025</v>
+        <v>13.7</v>
       </c>
       <c r="N8" t="n">
-        <v>0.0137</v>
-      </c>
-      <c r="O8" t="n">
-        <v>0.0015</v>
-      </c>
-      <c r="P8" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>0.0016</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -11897,52 +11567,43 @@
         <v>30</v>
       </c>
       <c r="B9" t="n">
-        <v>0.004</v>
+        <v>4</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0012</v>
+        <v>1.21</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0039</v>
+        <v>3.9</v>
       </c>
       <c r="E9" t="n">
-        <v>0.0011</v>
+        <v>1.1</v>
       </c>
       <c r="F9" t="n">
-        <v>0.007</v>
+        <v>7</v>
       </c>
       <c r="G9" t="n">
-        <v>0.0023</v>
+        <v>2.28</v>
       </c>
       <c r="H9" t="n">
-        <v>0.0048</v>
+        <v>4.8</v>
       </c>
       <c r="I9" t="n">
-        <v>0.0012</v>
+        <v>1.22</v>
       </c>
       <c r="J9" t="n">
-        <v>0.005</v>
+        <v>5</v>
       </c>
       <c r="K9" t="n">
-        <v>0.0016</v>
+        <v>1.65</v>
       </c>
       <c r="L9" t="n">
-        <v>0.0078</v>
+        <v>7.8</v>
       </c>
       <c r="M9" t="n">
-        <v>0.0037</v>
+        <v>10.1</v>
       </c>
       <c r="N9" t="n">
-        <v>0.0101</v>
-      </c>
-      <c r="O9" t="n">
-        <v>0.0018</v>
-      </c>
-      <c r="P9" t="n">
-        <v>0.017</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>0.0009</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10">
@@ -11950,52 +11611,43 @@
         <v>31</v>
       </c>
       <c r="B10" t="n">
-        <v>0.0081</v>
+        <v>8.1</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0029</v>
+        <v>2.92</v>
       </c>
       <c r="D10" t="n">
-        <v>0.01</v>
+        <v>10</v>
       </c>
       <c r="E10" t="n">
-        <v>0.0016</v>
+        <v>1.65</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0071</v>
+        <v>7.1</v>
       </c>
       <c r="G10" t="n">
-        <v>0.0054</v>
+        <v>5.45</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0038</v>
+        <v>3.8</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0045</v>
+        <v>4.46</v>
       </c>
       <c r="J10" t="n">
-        <v>0.0078</v>
+        <v>7.8</v>
       </c>
       <c r="K10" t="n">
-        <v>0.0038</v>
+        <v>3.82</v>
       </c>
       <c r="L10" t="n">
-        <v>0.0141</v>
+        <v>14.1</v>
       </c>
       <c r="M10" t="n">
-        <v>0.002</v>
+        <v>10.3</v>
       </c>
       <c r="N10" t="n">
-        <v>0.0103</v>
-      </c>
-      <c r="O10" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="P10" t="n">
-        <v>0</v>
-      </c>
-      <c r="Q10" t="n">
-        <v>0.0005</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -12003,52 +11655,43 @@
         <v>32</v>
       </c>
       <c r="B11" t="n">
-        <v>0.0094</v>
+        <v>9.4</v>
       </c>
       <c r="C11" t="n">
-        <v>0.006</v>
+        <v>6.01</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0089</v>
+        <v>8.9</v>
       </c>
       <c r="E11" t="n">
-        <v>0.0032</v>
+        <v>3.21</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0134</v>
+        <v>13.4</v>
       </c>
       <c r="G11" t="n">
-        <v>0.0053</v>
+        <v>5.31</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0106</v>
+        <v>10.6</v>
       </c>
       <c r="I11" t="n">
-        <v>0.0094</v>
+        <v>9.39</v>
       </c>
       <c r="J11" t="n">
-        <v>0.0111</v>
+        <v>11.1</v>
       </c>
       <c r="K11" t="n">
-        <v>0.0049</v>
+        <v>4.88</v>
       </c>
       <c r="L11" t="n">
-        <v>0.0056</v>
+        <v>5.6</v>
       </c>
       <c r="M11" t="n">
-        <v>0.0057</v>
+        <v>7.4</v>
       </c>
       <c r="N11" t="n">
-        <v>0.0074</v>
-      </c>
-      <c r="O11" t="n">
-        <v>0.0051</v>
-      </c>
-      <c r="P11" t="n">
-        <v>0.0194</v>
-      </c>
-      <c r="Q11" t="n">
-        <v>0.0023</v>
+        <v>19.4</v>
       </c>
     </row>
     <row r="12">
@@ -12057,36 +11700,27 @@
       </c>
       <c r="B12"/>
       <c r="C12" t="n">
-        <v>0.0053</v>
+        <v>5.29</v>
       </c>
       <c r="D12"/>
       <c r="E12" t="n">
-        <v>0.007</v>
+        <v>7.04</v>
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>0.007</v>
+        <v>7.01</v>
       </c>
       <c r="H12"/>
       <c r="I12" t="n">
-        <v>0.0068</v>
+        <v>6.76</v>
       </c>
       <c r="J12"/>
       <c r="K12" t="n">
-        <v>0.0069</v>
+        <v>6.88</v>
       </c>
       <c r="L12"/>
-      <c r="M12" t="n">
-        <v>0.0058</v>
-      </c>
+      <c r="M12"/>
       <c r="N12"/>
-      <c r="O12" t="n">
-        <v>0.0032</v>
-      </c>
-      <c r="P12"/>
-      <c r="Q12" t="n">
-        <v>0.0017</v>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -12094,36 +11728,27 @@
       </c>
       <c r="B13"/>
       <c r="C13" t="n">
-        <v>0.0068</v>
+        <v>6.81</v>
       </c>
       <c r="D13"/>
       <c r="E13" t="n">
-        <v>0.0061</v>
+        <v>6.09</v>
       </c>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>0.0082</v>
+        <v>8.2</v>
       </c>
       <c r="H13"/>
       <c r="I13" t="n">
-        <v>0.0089</v>
+        <v>8.86</v>
       </c>
       <c r="J13"/>
       <c r="K13" t="n">
-        <v>0.0074</v>
+        <v>7.36</v>
       </c>
       <c r="L13"/>
-      <c r="M13" t="n">
-        <v>0.0033</v>
-      </c>
+      <c r="M13"/>
       <c r="N13"/>
-      <c r="O13" t="n">
-        <v>0.0092</v>
-      </c>
-      <c r="P13"/>
-      <c r="Q13" t="n">
-        <v>0.003</v>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -12131,36 +11756,27 @@
       </c>
       <c r="B14"/>
       <c r="C14" t="n">
-        <v>0.0047</v>
+        <v>4.72</v>
       </c>
       <c r="D14"/>
       <c r="E14" t="n">
-        <v>0.0077</v>
+        <v>7.68</v>
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>0.014</v>
+        <v>14.05</v>
       </c>
       <c r="H14"/>
       <c r="I14" t="n">
-        <v>0.0116</v>
+        <v>11.61</v>
       </c>
       <c r="J14"/>
       <c r="K14" t="n">
-        <v>0.0083</v>
+        <v>8.33</v>
       </c>
       <c r="L14"/>
-      <c r="M14" t="n">
-        <v>0.007</v>
-      </c>
+      <c r="M14"/>
       <c r="N14"/>
-      <c r="O14" t="n">
-        <v>0.0033</v>
-      </c>
-      <c r="P14"/>
-      <c r="Q14" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -12168,36 +11784,27 @@
       </c>
       <c r="B15"/>
       <c r="C15" t="n">
-        <v>0.0099</v>
+        <v>9.9</v>
       </c>
       <c r="D15"/>
       <c r="E15" t="n">
-        <v>0.0026</v>
+        <v>2.6</v>
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>0.0059</v>
+        <v>5.9</v>
       </c>
       <c r="H15"/>
       <c r="I15" t="n">
-        <v>0.0075</v>
+        <v>7.49</v>
       </c>
       <c r="J15"/>
       <c r="K15" t="n">
-        <v>0.0045</v>
+        <v>4.49</v>
       </c>
       <c r="L15"/>
-      <c r="M15" t="n">
-        <v>0.0203</v>
-      </c>
+      <c r="M15"/>
       <c r="N15"/>
-      <c r="O15" t="n">
-        <v>0</v>
-      </c>
-      <c r="P15"/>
-      <c r="Q15" t="n">
-        <v>0</v>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -12205,15 +11812,15 @@
       </c>
       <c r="B16"/>
       <c r="C16" t="n">
-        <v>0.0033</v>
+        <v>3.34</v>
       </c>
       <c r="D16"/>
       <c r="E16" t="n">
-        <v>0.0026</v>
+        <v>2.62</v>
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>0.0018</v>
+        <v>1.77</v>
       </c>
       <c r="H16"/>
       <c r="I16" t="n">
@@ -12221,20 +11828,11 @@
       </c>
       <c r="J16"/>
       <c r="K16" t="n">
-        <v>0.0028</v>
+        <v>2.84</v>
       </c>
       <c r="L16"/>
-      <c r="M16" t="n">
-        <v>0</v>
-      </c>
+      <c r="M16"/>
       <c r="N16"/>
-      <c r="O16" t="n">
-        <v>0</v>
-      </c>
-      <c r="P16"/>
-      <c r="Q16" t="n">
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>